<commit_message>
Realizado todos los Metodos de Regresion Falta preguntar de la de Crecimiento
</commit_message>
<xml_diff>
--- a/Metodo Regresion Lineal MC.xlsx
+++ b/Metodo Regresion Lineal MC.xlsx
@@ -8,12 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Desktop\Analisis Numerico Git\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4493C9B3-827F-4177-87AF-A9D12592653D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DD29512-FAD9-453D-BF8C-FC1BC03BE820}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{7352DA56-3DAD-4B0F-ACAC-40C610105B66}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{7352DA56-3DAD-4B0F-ACAC-40C610105B66}"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Metodo Lineal" sheetId="1" r:id="rId1"/>
+    <sheet name="Metodo Exponencial" sheetId="2" r:id="rId2"/>
+    <sheet name="Metodo Potencia" sheetId="3" r:id="rId3"/>
+    <sheet name="Metodo Crecimiento" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -25,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="25">
   <si>
     <t>Xi</t>
   </si>
@@ -61,6 +64,45 @@
   </si>
   <si>
     <t>//&lt;-Si requiero Ampliar el Rango Recordar llevarlo a uno Menos que la Sumatoria</t>
+  </si>
+  <si>
+    <t>Ln(Yi)</t>
+  </si>
+  <si>
+    <t>Xi*ln(Yi)</t>
+  </si>
+  <si>
+    <t>B:</t>
+  </si>
+  <si>
+    <t>A:</t>
+  </si>
+  <si>
+    <t>//&lt;- Seria cambiarle la posicion de la sumatoria a A1 y A2.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">//&lt;- La posicion de la sumatoria </t>
+  </si>
+  <si>
+    <t xml:space="preserve">//&lt;- Es la sumatoria, para no confundirse </t>
+  </si>
+  <si>
+    <t>Log(Yi)</t>
+  </si>
+  <si>
+    <t>Log(Xi)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Log(Xi)*Log(Yi)</t>
+  </si>
+  <si>
+    <t>1/Xi</t>
+  </si>
+  <si>
+    <t>(1/Xi)*(1/Yi)</t>
+  </si>
+  <si>
+    <t>&lt;-Como Se Denota la RTA?????</t>
   </si>
 </sst>
 </file>
@@ -295,7 +337,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -312,7 +354,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -360,7 +402,7 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -369,6 +411,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -685,8 +741,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36ABAA54-3098-44BF-93C5-BB384424DD94}">
   <dimension ref="F1:U21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="M20" sqref="M20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="T8" sqref="T8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -916,6 +972,12 @@
       <c r="K11" s="1"/>
       <c r="L11" s="1"/>
       <c r="M11" s="1"/>
+      <c r="O11" s="27" t="s">
+        <v>18</v>
+      </c>
+      <c r="P11" s="27"/>
+      <c r="Q11" s="27"/>
+      <c r="R11" s="27"/>
     </row>
     <row r="12" spans="6:21" x14ac:dyDescent="0.25">
       <c r="F12" s="5"/>
@@ -1035,4 +1097,1577 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8AA40654-A814-40D2-871E-188E3E9FF765}">
+  <dimension ref="F1:V22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N15" sqref="N15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="10" max="10" width="11.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="6:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F1" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="18"/>
+    </row>
+    <row r="2" spans="6:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J2" s="1"/>
+      <c r="M2" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="N2" s="1"/>
+      <c r="O2" s="1"/>
+    </row>
+    <row r="3" spans="6:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="M3" s="12">
+        <f>COUNTA(F4:F20)</f>
+        <v>5</v>
+      </c>
+      <c r="N3" s="1"/>
+      <c r="O3" s="1"/>
+      <c r="P3" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q3" s="27"/>
+      <c r="R3" s="27"/>
+      <c r="S3" s="27"/>
+      <c r="T3" s="27"/>
+      <c r="U3" s="27"/>
+      <c r="V3" s="27"/>
+    </row>
+    <row r="4" spans="6:22" x14ac:dyDescent="0.25">
+      <c r="F4" s="5">
+        <v>1</v>
+      </c>
+      <c r="G4" s="30">
+        <v>0.5</v>
+      </c>
+      <c r="H4" s="30">
+        <f>IF(G4 &gt; 0, LN(G4), 0)</f>
+        <v>-0.69314718055994529</v>
+      </c>
+      <c r="I4" s="30">
+        <f>F4*F4</f>
+        <v>1</v>
+      </c>
+      <c r="J4" s="7">
+        <f>F4*H4</f>
+        <v>-0.69314718055994529</v>
+      </c>
+      <c r="M4" s="1"/>
+      <c r="N4" s="1"/>
+      <c r="O4" s="1"/>
+    </row>
+    <row r="5" spans="6:22" x14ac:dyDescent="0.25">
+      <c r="F5" s="5">
+        <v>2</v>
+      </c>
+      <c r="G5" s="30">
+        <v>1.7</v>
+      </c>
+      <c r="H5" s="30">
+        <f t="shared" ref="H5:H20" si="0">IF(G5 &gt; 0, LN(G5), 0)</f>
+        <v>0.53062825106217038</v>
+      </c>
+      <c r="I5" s="30">
+        <f>F5*F5</f>
+        <v>4</v>
+      </c>
+      <c r="J5" s="7">
+        <f t="shared" ref="J5:J20" si="1">F5*H5</f>
+        <v>1.0612565021243408</v>
+      </c>
+      <c r="M5" s="1"/>
+      <c r="N5" s="1"/>
+      <c r="O5" s="1"/>
+    </row>
+    <row r="6" spans="6:22" x14ac:dyDescent="0.25">
+      <c r="F6" s="5">
+        <v>3</v>
+      </c>
+      <c r="G6" s="30">
+        <v>3.4</v>
+      </c>
+      <c r="H6" s="30">
+        <f t="shared" si="0"/>
+        <v>1.2237754316221157</v>
+      </c>
+      <c r="I6" s="30">
+        <f>F6*F6</f>
+        <v>9</v>
+      </c>
+      <c r="J6" s="7">
+        <f t="shared" si="1"/>
+        <v>3.671326294866347</v>
+      </c>
+      <c r="M6" s="1"/>
+      <c r="N6" s="1"/>
+      <c r="O6" s="1"/>
+    </row>
+    <row r="7" spans="6:22" x14ac:dyDescent="0.25">
+      <c r="F7" s="5">
+        <v>4</v>
+      </c>
+      <c r="G7" s="30">
+        <v>5.7</v>
+      </c>
+      <c r="H7" s="30">
+        <f t="shared" si="0"/>
+        <v>1.7404661748405046</v>
+      </c>
+      <c r="I7" s="30">
+        <f>F7*F7</f>
+        <v>16</v>
+      </c>
+      <c r="J7" s="7">
+        <f t="shared" si="1"/>
+        <v>6.9618646993620183</v>
+      </c>
+      <c r="M7" s="1"/>
+      <c r="N7" s="29"/>
+      <c r="O7" s="1"/>
+    </row>
+    <row r="8" spans="6:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F8" s="5">
+        <v>5</v>
+      </c>
+      <c r="G8" s="30">
+        <v>8.4</v>
+      </c>
+      <c r="H8" s="30">
+        <f t="shared" si="0"/>
+        <v>2.1282317058492679</v>
+      </c>
+      <c r="I8" s="30">
+        <f>F8*F8</f>
+        <v>25</v>
+      </c>
+      <c r="J8" s="7">
+        <f t="shared" si="1"/>
+        <v>10.64115852924634</v>
+      </c>
+      <c r="M8" s="1"/>
+      <c r="N8" s="1"/>
+      <c r="O8" s="1"/>
+    </row>
+    <row r="9" spans="6:22" x14ac:dyDescent="0.25">
+      <c r="F9" s="5"/>
+      <c r="G9" s="30"/>
+      <c r="H9" s="30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I9" s="30">
+        <f>F9*F9</f>
+        <v>0</v>
+      </c>
+      <c r="J9" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M9" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="N9" s="1"/>
+      <c r="O9" s="14" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="6:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F10" s="5"/>
+      <c r="G10" s="30"/>
+      <c r="H10" s="30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I10" s="30">
+        <f>F10*F10</f>
+        <v>0</v>
+      </c>
+      <c r="J10" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M10" s="12">
+        <f>((M3*J21)-(F21*H21))/((M3*I21)-(F21*F21))</f>
+        <v>0.68525956965967627</v>
+      </c>
+      <c r="N10" s="1"/>
+      <c r="O10" s="12">
+        <f>(H21/M3)-M10*(F21/M3)</f>
+        <v>-1.0697878324162062</v>
+      </c>
+      <c r="Q10" s="27" t="s">
+        <v>9</v>
+      </c>
+      <c r="R10" s="27"/>
+      <c r="S10" s="27"/>
+      <c r="T10" s="27"/>
+      <c r="U10" s="27"/>
+      <c r="V10" s="27"/>
+    </row>
+    <row r="11" spans="6:22" x14ac:dyDescent="0.25">
+      <c r="F11" s="5"/>
+      <c r="G11" s="30"/>
+      <c r="H11" s="30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I11" s="30">
+        <f>F11*F11</f>
+        <v>0</v>
+      </c>
+      <c r="J11" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M11" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="N11" s="1"/>
+      <c r="O11" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q11" s="27" t="s">
+        <v>17</v>
+      </c>
+      <c r="R11" s="27"/>
+      <c r="S11" s="27"/>
+    </row>
+    <row r="12" spans="6:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F12" s="5"/>
+      <c r="G12" s="30"/>
+      <c r="H12" s="30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I12" s="30">
+        <f>F12*F12</f>
+        <v>0</v>
+      </c>
+      <c r="J12" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M12" s="12">
+        <f>M10</f>
+        <v>0.68525956965967627</v>
+      </c>
+      <c r="N12" s="1"/>
+      <c r="O12" s="12">
+        <f>EXP(O10)</f>
+        <v>0.34308130042789264</v>
+      </c>
+    </row>
+    <row r="13" spans="6:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F13" s="5"/>
+      <c r="G13" s="30"/>
+      <c r="H13" s="30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I13" s="30">
+        <f>F13*F13</f>
+        <v>0</v>
+      </c>
+      <c r="J13" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M13" s="1"/>
+      <c r="N13" s="1"/>
+      <c r="O13" s="1"/>
+    </row>
+    <row r="14" spans="6:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F14" s="23"/>
+      <c r="G14" s="31"/>
+      <c r="H14" s="30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I14" s="30">
+        <f>F14*F14</f>
+        <v>0</v>
+      </c>
+      <c r="J14" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M14" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="N14" s="20" t="str">
+        <f>"Y = "&amp;O12&amp;" * e  ^("&amp;M12&amp;")"</f>
+        <v>Y = 0,343081300427893 * e  ^(0,685259569659676)</v>
+      </c>
+      <c r="O14" s="21"/>
+      <c r="P14" s="20"/>
+      <c r="Q14" s="22"/>
+    </row>
+    <row r="15" spans="6:22" x14ac:dyDescent="0.25">
+      <c r="F15" s="23"/>
+      <c r="G15" s="31"/>
+      <c r="H15" s="30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I15" s="30">
+        <f>F15*F15</f>
+        <v>0</v>
+      </c>
+      <c r="J15" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="6:22" x14ac:dyDescent="0.25">
+      <c r="F16" s="23"/>
+      <c r="G16" s="31"/>
+      <c r="H16" s="30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I16" s="30">
+        <f>F16*F16</f>
+        <v>0</v>
+      </c>
+      <c r="J16" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="6:19" x14ac:dyDescent="0.25">
+      <c r="F17" s="23"/>
+      <c r="G17" s="31"/>
+      <c r="H17" s="30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I17" s="30">
+        <f>F17*F17</f>
+        <v>0</v>
+      </c>
+      <c r="J17" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="6:19" x14ac:dyDescent="0.25">
+      <c r="F18" s="23"/>
+      <c r="G18" s="31"/>
+      <c r="H18" s="30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I18" s="30">
+        <f>F18*F18</f>
+        <v>0</v>
+      </c>
+      <c r="J18" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="6:19" x14ac:dyDescent="0.25">
+      <c r="F19" s="23"/>
+      <c r="G19" s="31"/>
+      <c r="H19" s="30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I19" s="30">
+        <f>F19*F19</f>
+        <v>0</v>
+      </c>
+      <c r="J19" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="6:19" x14ac:dyDescent="0.25">
+      <c r="F20" s="23"/>
+      <c r="G20" s="31"/>
+      <c r="H20" s="30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I20" s="30">
+        <f>F20*F20</f>
+        <v>0</v>
+      </c>
+      <c r="J20" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="O20" s="28"/>
+    </row>
+    <row r="21" spans="6:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F21" s="8">
+        <f t="shared" ref="F21:I21" si="2">SUM(F4:F20)</f>
+        <v>15</v>
+      </c>
+      <c r="G21" s="9">
+        <f t="shared" si="2"/>
+        <v>19.700000000000003</v>
+      </c>
+      <c r="H21" s="9">
+        <f t="shared" ref="H21" si="3">SUM(H4:H20)</f>
+        <v>4.9299543828141132</v>
+      </c>
+      <c r="I21" s="9">
+        <f>SUM(I4:I20)</f>
+        <v>55</v>
+      </c>
+      <c r="J21" s="10">
+        <f>SUM(J4:J20)</f>
+        <v>21.642458845039101</v>
+      </c>
+      <c r="M21" s="27" t="s">
+        <v>10</v>
+      </c>
+      <c r="N21" s="27"/>
+      <c r="O21" s="27"/>
+      <c r="P21" s="27"/>
+      <c r="Q21" s="27"/>
+      <c r="R21" s="27"/>
+      <c r="S21" s="27"/>
+    </row>
+    <row r="22" spans="6:19" x14ac:dyDescent="0.25">
+      <c r="M22" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="N22" s="27"/>
+      <c r="O22" s="27"/>
+      <c r="P22" s="27"/>
+      <c r="Q22" s="27"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF479F44-E340-4DDF-A0A6-FFCC584E9C63}">
+  <dimension ref="E1:W22"/>
+  <sheetViews>
+    <sheetView topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1:W22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="15" max="15" width="11.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="5:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F1" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="18"/>
+    </row>
+    <row r="2" spans="5:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J2" s="1"/>
+      <c r="M2" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="N2" s="1"/>
+      <c r="O2" s="1"/>
+    </row>
+    <row r="3" spans="5:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F3" s="32" t="s">
+        <v>20</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="M3" s="12">
+        <f>COUNTA(E4:E20)</f>
+        <v>5</v>
+      </c>
+      <c r="N3" s="1"/>
+      <c r="O3" s="1"/>
+      <c r="P3" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q3" s="27"/>
+      <c r="R3" s="27"/>
+      <c r="S3" s="27"/>
+      <c r="T3" s="27"/>
+      <c r="U3" s="27"/>
+      <c r="V3" s="27"/>
+    </row>
+    <row r="4" spans="5:23" x14ac:dyDescent="0.25">
+      <c r="E4" s="5">
+        <v>1</v>
+      </c>
+      <c r="F4" s="33">
+        <f>IF(E4 &gt; 0, LOG(E4), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="G4" s="30">
+        <v>0.5</v>
+      </c>
+      <c r="H4" s="30">
+        <f>IF(G4 &gt; 0, LOG(G4), 0)</f>
+        <v>-0.3010299956639812</v>
+      </c>
+      <c r="I4" s="30">
+        <f>F4*F4</f>
+        <v>0</v>
+      </c>
+      <c r="J4" s="7">
+        <f>F4*H4</f>
+        <v>0</v>
+      </c>
+      <c r="K4" s="28"/>
+      <c r="M4" s="1"/>
+      <c r="N4" s="1"/>
+      <c r="O4" s="1"/>
+    </row>
+    <row r="5" spans="5:23" x14ac:dyDescent="0.25">
+      <c r="E5" s="5">
+        <v>2</v>
+      </c>
+      <c r="F5" s="33">
+        <f t="shared" ref="F5:F20" si="0">IF(E5 &gt; 0, LOG(E5), 0)</f>
+        <v>0.3010299956639812</v>
+      </c>
+      <c r="G5" s="30">
+        <v>1.7</v>
+      </c>
+      <c r="H5" s="30">
+        <f t="shared" ref="H5:H20" si="1">IF(G5 &gt; 0, LOG(G5), 0)</f>
+        <v>0.23044892137827391</v>
+      </c>
+      <c r="I5" s="30">
+        <f t="shared" ref="I5:I20" si="2">F5*F5</f>
+        <v>9.0619058289456544E-2</v>
+      </c>
+      <c r="J5" s="7">
+        <f t="shared" ref="J5:J20" si="3">F5*H5</f>
+        <v>6.9372037803270933E-2</v>
+      </c>
+      <c r="M5" s="1"/>
+      <c r="N5" s="1"/>
+      <c r="O5" s="1"/>
+    </row>
+    <row r="6" spans="5:23" x14ac:dyDescent="0.25">
+      <c r="E6" s="5">
+        <v>3</v>
+      </c>
+      <c r="F6" s="33">
+        <f t="shared" si="0"/>
+        <v>0.47712125471966244</v>
+      </c>
+      <c r="G6" s="30">
+        <v>3.4</v>
+      </c>
+      <c r="H6" s="30">
+        <f t="shared" si="1"/>
+        <v>0.53147891704225514</v>
+      </c>
+      <c r="I6" s="30">
+        <f t="shared" si="2"/>
+        <v>0.227644691705265</v>
+      </c>
+      <c r="J6" s="7">
+        <f t="shared" si="3"/>
+        <v>0.25357988775624818</v>
+      </c>
+      <c r="M6" s="1"/>
+      <c r="N6" s="1"/>
+      <c r="O6" s="1"/>
+    </row>
+    <row r="7" spans="5:23" x14ac:dyDescent="0.25">
+      <c r="E7" s="5">
+        <v>4</v>
+      </c>
+      <c r="F7" s="33">
+        <f t="shared" si="0"/>
+        <v>0.6020599913279624</v>
+      </c>
+      <c r="G7" s="30">
+        <v>5.7</v>
+      </c>
+      <c r="H7" s="30">
+        <f t="shared" si="1"/>
+        <v>0.75587485567249146</v>
+      </c>
+      <c r="I7" s="30">
+        <f t="shared" si="2"/>
+        <v>0.36247623315782618</v>
+      </c>
+      <c r="J7" s="7">
+        <f t="shared" si="3"/>
+        <v>0.45508200905120505</v>
+      </c>
+      <c r="M7" s="1"/>
+      <c r="N7" s="29"/>
+      <c r="O7" s="1"/>
+    </row>
+    <row r="8" spans="5:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E8" s="5">
+        <v>5</v>
+      </c>
+      <c r="F8" s="33">
+        <f t="shared" si="0"/>
+        <v>0.69897000433601886</v>
+      </c>
+      <c r="G8" s="30">
+        <v>8.4</v>
+      </c>
+      <c r="H8" s="30">
+        <f t="shared" si="1"/>
+        <v>0.9242792860618817</v>
+      </c>
+      <c r="I8" s="30">
+        <f t="shared" si="2"/>
+        <v>0.4885590669614942</v>
+      </c>
+      <c r="J8" s="7">
+        <f t="shared" si="3"/>
+        <v>0.64604349658636584</v>
+      </c>
+      <c r="M8" s="1"/>
+      <c r="N8" s="1"/>
+      <c r="O8" s="1"/>
+    </row>
+    <row r="9" spans="5:23" x14ac:dyDescent="0.25">
+      <c r="E9" s="5"/>
+      <c r="F9" s="33">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G9" s="30"/>
+      <c r="H9" s="30">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I9" s="30">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J9" s="7">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="M9" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="N9" s="1"/>
+      <c r="O9" s="14" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="5:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E10" s="5"/>
+      <c r="F10" s="33">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G10" s="30"/>
+      <c r="H10" s="30">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I10" s="30">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J10" s="7">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="M10" s="12">
+        <f>((M3*J21)-(F21*H21))/((M3*I21)-(F21*F21))</f>
+        <v>1.7517236480773599</v>
+      </c>
+      <c r="N10" s="1"/>
+      <c r="O10" s="12">
+        <f>(H21/M3)-M10*(F21/M3)</f>
+        <v>-0.30021979456993098</v>
+      </c>
+      <c r="Q10" s="27" t="s">
+        <v>9</v>
+      </c>
+      <c r="R10" s="27"/>
+      <c r="S10" s="27"/>
+      <c r="T10" s="27"/>
+      <c r="U10" s="27"/>
+      <c r="V10" s="27"/>
+      <c r="W10" s="27"/>
+    </row>
+    <row r="11" spans="5:23" x14ac:dyDescent="0.25">
+      <c r="E11" s="5"/>
+      <c r="F11" s="33">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G11" s="30"/>
+      <c r="H11" s="30">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I11" s="30">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J11" s="7">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="M11" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="N11" s="1"/>
+      <c r="O11" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q11" s="27" t="s">
+        <v>17</v>
+      </c>
+      <c r="R11" s="27"/>
+      <c r="S11" s="27"/>
+    </row>
+    <row r="12" spans="5:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E12" s="5"/>
+      <c r="F12" s="33">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G12" s="30"/>
+      <c r="H12" s="30">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I12" s="30">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J12" s="7">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="M12" s="12">
+        <f>M10</f>
+        <v>1.7517236480773599</v>
+      </c>
+      <c r="N12" s="1"/>
+      <c r="O12" s="12">
+        <f>POWER(10,O10)</f>
+        <v>0.50093364909774885</v>
+      </c>
+    </row>
+    <row r="13" spans="5:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E13" s="5"/>
+      <c r="F13" s="33">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G13" s="30"/>
+      <c r="H13" s="30">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I13" s="30">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J13" s="7">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="M13" s="1"/>
+      <c r="N13" s="1"/>
+      <c r="O13" s="1"/>
+    </row>
+    <row r="14" spans="5:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E14" s="23"/>
+      <c r="F14" s="33">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G14" s="31"/>
+      <c r="H14" s="30">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I14" s="30">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J14" s="7">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="M14" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="N14" s="20" t="str">
+        <f>"Y = "&amp;O12&amp;" * x  ^("&amp;M12&amp;")"</f>
+        <v>Y = 0,500933649097749 * x  ^(1,75172364807736)</v>
+      </c>
+      <c r="O14" s="21"/>
+      <c r="P14" s="20"/>
+      <c r="Q14" s="22"/>
+    </row>
+    <row r="15" spans="5:23" x14ac:dyDescent="0.25">
+      <c r="E15" s="23"/>
+      <c r="F15" s="33">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G15" s="31"/>
+      <c r="H15" s="30">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I15" s="30">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J15" s="7">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="5:23" x14ac:dyDescent="0.25">
+      <c r="E16" s="23"/>
+      <c r="F16" s="33">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G16" s="31"/>
+      <c r="H16" s="30">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I16" s="30">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J16" s="7">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="5:19" x14ac:dyDescent="0.25">
+      <c r="E17" s="23"/>
+      <c r="F17" s="33">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G17" s="31"/>
+      <c r="H17" s="30">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I17" s="30">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J17" s="7">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="5:19" x14ac:dyDescent="0.25">
+      <c r="E18" s="23"/>
+      <c r="F18" s="33">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G18" s="31"/>
+      <c r="H18" s="30">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I18" s="30">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J18" s="7">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="5:19" x14ac:dyDescent="0.25">
+      <c r="E19" s="23"/>
+      <c r="F19" s="33">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G19" s="31"/>
+      <c r="H19" s="30">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I19" s="30">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J19" s="7">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="5:19" x14ac:dyDescent="0.25">
+      <c r="E20" s="23"/>
+      <c r="F20" s="33">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G20" s="31"/>
+      <c r="H20" s="30">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I20" s="30">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J20" s="7">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="O20" s="28"/>
+    </row>
+    <row r="21" spans="5:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E21" s="8">
+        <f>SUM(E4:E20)</f>
+        <v>15</v>
+      </c>
+      <c r="F21" s="34">
+        <f>SUM(F4:F20)</f>
+        <v>2.0791812460476247</v>
+      </c>
+      <c r="G21" s="9">
+        <f>SUM(G4:G20)</f>
+        <v>19.700000000000003</v>
+      </c>
+      <c r="H21" s="9">
+        <f t="shared" ref="H21" si="4">SUM(H4:H20)</f>
+        <v>2.1410519844909208</v>
+      </c>
+      <c r="I21" s="9">
+        <f>SUM(I4:I20)</f>
+        <v>1.1692990501140419</v>
+      </c>
+      <c r="J21" s="10">
+        <f>SUM(J4:J20)</f>
+        <v>1.4240774311970901</v>
+      </c>
+      <c r="M21" s="27" t="s">
+        <v>10</v>
+      </c>
+      <c r="N21" s="27"/>
+      <c r="O21" s="27"/>
+      <c r="P21" s="27"/>
+      <c r="Q21" s="27"/>
+      <c r="R21" s="27"/>
+      <c r="S21" s="27"/>
+    </row>
+    <row r="22" spans="5:19" x14ac:dyDescent="0.25">
+      <c r="M22" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="N22" s="27"/>
+      <c r="O22" s="27"/>
+      <c r="P22" s="27"/>
+      <c r="Q22" s="27"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{803B4C9E-8A60-4D57-AACF-2E84BA4F73FE}">
+  <dimension ref="E1:W22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L7" sqref="L7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="5:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F1" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="18"/>
+    </row>
+    <row r="2" spans="5:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J2" s="1"/>
+      <c r="M2" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="N2" s="1"/>
+      <c r="O2" s="1"/>
+    </row>
+    <row r="3" spans="5:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F3" s="32" t="s">
+        <v>22</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="M3" s="12">
+        <f>COUNTA(E4:E20)</f>
+        <v>5</v>
+      </c>
+      <c r="N3" s="1"/>
+      <c r="O3" s="1"/>
+      <c r="P3" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q3" s="27"/>
+      <c r="R3" s="27"/>
+      <c r="S3" s="27"/>
+      <c r="T3" s="27"/>
+      <c r="U3" s="27"/>
+      <c r="V3" s="27"/>
+    </row>
+    <row r="4" spans="5:23" x14ac:dyDescent="0.25">
+      <c r="E4" s="5">
+        <v>1</v>
+      </c>
+      <c r="F4" s="33">
+        <f>IF(E4 &gt; 0,1/E4, 0)</f>
+        <v>1</v>
+      </c>
+      <c r="G4" s="30">
+        <v>0.5</v>
+      </c>
+      <c r="H4" s="30">
+        <f>IF(G4 &gt; 0, 1/G4, 0)</f>
+        <v>2</v>
+      </c>
+      <c r="I4" s="30">
+        <f>F4*F4</f>
+        <v>1</v>
+      </c>
+      <c r="J4" s="7">
+        <f>F4*H4</f>
+        <v>2</v>
+      </c>
+      <c r="K4" s="28"/>
+      <c r="M4" s="1"/>
+      <c r="N4" s="1"/>
+      <c r="O4" s="1"/>
+    </row>
+    <row r="5" spans="5:23" x14ac:dyDescent="0.25">
+      <c r="E5" s="5">
+        <v>2</v>
+      </c>
+      <c r="F5" s="33">
+        <f t="shared" ref="F5:F20" si="0">IF(E5 &gt; 0,1/E5, 0)</f>
+        <v>0.5</v>
+      </c>
+      <c r="G5" s="30">
+        <v>1.7</v>
+      </c>
+      <c r="H5" s="30">
+        <f t="shared" ref="H5:H20" si="1">IF(G5 &gt; 0, 1/G5, 0)</f>
+        <v>0.58823529411764708</v>
+      </c>
+      <c r="I5" s="30">
+        <f t="shared" ref="I5:I20" si="2">F5*F5</f>
+        <v>0.25</v>
+      </c>
+      <c r="J5" s="7">
+        <f t="shared" ref="J5:J20" si="3">F5*H5</f>
+        <v>0.29411764705882354</v>
+      </c>
+      <c r="M5" s="1"/>
+      <c r="N5" s="1"/>
+      <c r="O5" s="1"/>
+    </row>
+    <row r="6" spans="5:23" x14ac:dyDescent="0.25">
+      <c r="E6" s="5">
+        <v>3</v>
+      </c>
+      <c r="F6" s="33">
+        <f t="shared" si="0"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="G6" s="30">
+        <v>3.4</v>
+      </c>
+      <c r="H6" s="30">
+        <f t="shared" si="1"/>
+        <v>0.29411764705882354</v>
+      </c>
+      <c r="I6" s="30">
+        <f t="shared" si="2"/>
+        <v>0.1111111111111111</v>
+      </c>
+      <c r="J6" s="7">
+        <f t="shared" si="3"/>
+        <v>9.8039215686274508E-2</v>
+      </c>
+      <c r="M6" s="1"/>
+      <c r="N6" s="1"/>
+      <c r="O6" s="1"/>
+    </row>
+    <row r="7" spans="5:23" x14ac:dyDescent="0.25">
+      <c r="E7" s="5">
+        <v>4</v>
+      </c>
+      <c r="F7" s="33">
+        <f t="shared" si="0"/>
+        <v>0.25</v>
+      </c>
+      <c r="G7" s="30">
+        <v>5.7</v>
+      </c>
+      <c r="H7" s="30">
+        <f t="shared" si="1"/>
+        <v>0.17543859649122806</v>
+      </c>
+      <c r="I7" s="30">
+        <f t="shared" si="2"/>
+        <v>6.25E-2</v>
+      </c>
+      <c r="J7" s="7">
+        <f t="shared" si="3"/>
+        <v>4.3859649122807015E-2</v>
+      </c>
+      <c r="L7" s="28"/>
+      <c r="M7" s="1"/>
+      <c r="N7" s="29"/>
+      <c r="O7" s="1"/>
+    </row>
+    <row r="8" spans="5:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E8" s="5">
+        <v>5</v>
+      </c>
+      <c r="F8" s="33">
+        <f t="shared" si="0"/>
+        <v>0.2</v>
+      </c>
+      <c r="G8" s="30">
+        <v>8.4</v>
+      </c>
+      <c r="H8" s="30">
+        <f t="shared" si="1"/>
+        <v>0.11904761904761904</v>
+      </c>
+      <c r="I8" s="30">
+        <f t="shared" si="2"/>
+        <v>4.0000000000000008E-2</v>
+      </c>
+      <c r="J8" s="7">
+        <f t="shared" si="3"/>
+        <v>2.3809523809523808E-2</v>
+      </c>
+      <c r="M8" s="1"/>
+      <c r="N8" s="1"/>
+      <c r="O8" s="1"/>
+    </row>
+    <row r="9" spans="5:23" x14ac:dyDescent="0.25">
+      <c r="E9" s="5"/>
+      <c r="F9" s="33">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G9" s="30"/>
+      <c r="H9" s="30">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I9" s="30">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J9" s="7">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="M9" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="N9" s="1"/>
+      <c r="O9" s="14" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="5:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E10" s="5"/>
+      <c r="F10" s="33">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G10" s="30"/>
+      <c r="H10" s="30">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I10" s="30">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J10" s="7">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="M10" s="12">
+        <f>((M3*J21)-(F21*H21))/((M3*I21)-(F21*F21))</f>
+        <v>2.397472383050923</v>
+      </c>
+      <c r="N10" s="1"/>
+      <c r="O10" s="12">
+        <f>(H21/M3)-M10*(F21/M3)</f>
+        <v>-0.45947789025019126</v>
+      </c>
+      <c r="Q10" s="27" t="s">
+        <v>9</v>
+      </c>
+      <c r="R10" s="27"/>
+      <c r="S10" s="27"/>
+      <c r="T10" s="27"/>
+      <c r="U10" s="27"/>
+      <c r="V10" s="27"/>
+      <c r="W10" s="27"/>
+    </row>
+    <row r="11" spans="5:23" x14ac:dyDescent="0.25">
+      <c r="E11" s="5"/>
+      <c r="F11" s="33">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G11" s="30"/>
+      <c r="H11" s="30">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I11" s="30">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J11" s="7">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="M11" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="N11" s="1"/>
+      <c r="O11" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q11" s="27" t="s">
+        <v>17</v>
+      </c>
+      <c r="R11" s="27"/>
+      <c r="S11" s="27"/>
+    </row>
+    <row r="12" spans="5:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E12" s="5"/>
+      <c r="F12" s="33">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G12" s="30"/>
+      <c r="H12" s="30">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I12" s="30">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J12" s="7">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="M12" s="12">
+        <f>M10</f>
+        <v>2.397472383050923</v>
+      </c>
+      <c r="N12" s="1"/>
+      <c r="O12" s="12">
+        <f>POWER(10,O10)</f>
+        <v>0.34715394889967566</v>
+      </c>
+    </row>
+    <row r="13" spans="5:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E13" s="5"/>
+      <c r="F13" s="33">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G13" s="30"/>
+      <c r="H13" s="30">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I13" s="30">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J13" s="7">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="M13" s="1"/>
+      <c r="N13" s="1"/>
+      <c r="O13" s="1"/>
+    </row>
+    <row r="14" spans="5:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E14" s="23"/>
+      <c r="F14" s="33">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G14" s="31"/>
+      <c r="H14" s="30">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I14" s="30">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J14" s="7">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="M14" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="N14" s="20" t="str">
+        <f>"Y = "&amp;O12&amp;" * x  ^("&amp;M12&amp;")"</f>
+        <v>Y = 0,347153948899676 * x  ^(2,39747238305092)</v>
+      </c>
+      <c r="O14" s="21"/>
+      <c r="P14" s="20"/>
+      <c r="Q14" s="22"/>
+      <c r="S14" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="T14" s="27"/>
+      <c r="U14" s="27"/>
+    </row>
+    <row r="15" spans="5:23" x14ac:dyDescent="0.25">
+      <c r="E15" s="23"/>
+      <c r="F15" s="33">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G15" s="31"/>
+      <c r="H15" s="30">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I15" s="30">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J15" s="7">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="5:23" x14ac:dyDescent="0.25">
+      <c r="E16" s="23"/>
+      <c r="F16" s="33">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G16" s="31"/>
+      <c r="H16" s="30">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I16" s="30">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J16" s="7">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="5:19" x14ac:dyDescent="0.25">
+      <c r="E17" s="23"/>
+      <c r="F17" s="33">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G17" s="31"/>
+      <c r="H17" s="30">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I17" s="30">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J17" s="7">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="5:19" x14ac:dyDescent="0.25">
+      <c r="E18" s="23"/>
+      <c r="F18" s="33">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G18" s="31"/>
+      <c r="H18" s="30">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I18" s="30">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J18" s="7">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="5:19" x14ac:dyDescent="0.25">
+      <c r="E19" s="23"/>
+      <c r="F19" s="33">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G19" s="31"/>
+      <c r="H19" s="30">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I19" s="30">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J19" s="7">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="5:19" x14ac:dyDescent="0.25">
+      <c r="E20" s="23"/>
+      <c r="F20" s="33">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G20" s="31"/>
+      <c r="H20" s="30">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I20" s="30">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J20" s="7">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="O20" s="28"/>
+    </row>
+    <row r="21" spans="5:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E21" s="8">
+        <f>SUM(E4:E20)</f>
+        <v>15</v>
+      </c>
+      <c r="F21" s="34">
+        <f>SUM(F4:F20)</f>
+        <v>2.2833333333333332</v>
+      </c>
+      <c r="G21" s="9">
+        <f>SUM(G4:G20)</f>
+        <v>19.700000000000003</v>
+      </c>
+      <c r="H21" s="9">
+        <f t="shared" ref="H21" si="4">SUM(H4:H20)</f>
+        <v>3.1768391567153178</v>
+      </c>
+      <c r="I21" s="9">
+        <f>SUM(I4:I20)</f>
+        <v>1.4636111111111112</v>
+      </c>
+      <c r="J21" s="10">
+        <f>SUM(J4:J20)</f>
+        <v>2.4598260356774286</v>
+      </c>
+      <c r="M21" s="27" t="s">
+        <v>10</v>
+      </c>
+      <c r="N21" s="27"/>
+      <c r="O21" s="27"/>
+      <c r="P21" s="27"/>
+      <c r="Q21" s="27"/>
+      <c r="R21" s="27"/>
+      <c r="S21" s="27"/>
+    </row>
+    <row r="22" spans="5:19" x14ac:dyDescent="0.25">
+      <c r="M22" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="N22" s="27"/>
+      <c r="O22" s="27"/>
+      <c r="P22" s="27"/>
+      <c r="Q22" s="27"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>